<commit_message>
updated BOM excell file
</commit_message>
<xml_diff>
--- a/PCB/PCB_new/PCB_2020_BOM.xlsx
+++ b/PCB/PCB_new/PCB_2020_BOM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\Documents\AMP\AMP-19-20\PCB\PCB_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7D338F40-53BB-4391-85E7-A2E1A687C57E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3ACF24AD-990B-45DC-A8B6-0BF6D167425C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37845" yWindow="5535" windowWidth="19815" windowHeight="10320"/>
+    <workbookView xWindow="1116" yWindow="744" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_2020" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="120" uniqueCount="74">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="100" uniqueCount="73">
   <si>
     <t>Reference</t>
   </si>
@@ -150,9 +150,6 @@
     <t>https://www.digikey.com/product-detail/en/texas-instruments/LM358N-NOPB/LM358NNS-NOPB-ND/6264</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1 </t>
-  </si>
-  <si>
     <t>220mA/50V/3.5Î©</t>
   </si>
   <si>
@@ -174,21 +171,12 @@
     <t>https://www.infineon.com/dgdl/irl530npbf.pdf?fileId=5546d462533600a40153565fad5c2560</t>
   </si>
   <si>
-    <t xml:space="preserve">R1 R2 </t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
     <t>Resistor_SMD:R_0805_2012Metric_Pad1.15x1.40mm_HandSolder</t>
   </si>
   <si>
-    <t xml:space="preserve">R16 R17 </t>
-  </si>
-  <si>
-    <t>R-US_R0805</t>
-  </si>
-  <si>
     <t xml:space="preserve">R3 </t>
   </si>
   <si>
@@ -247,12 +235,21 @@
   </si>
   <si>
     <t>https://www.digikey.com/product-detail/en/3m/4808-3004-CP/3M5473-ND/1133626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1 R2 R6 R8 R7 R9 </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/826629-2/A105107-ND/1130753?utm_adgroup=Connectors%20&amp;%20Interconnects&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search&amp;utm_term=&amp;utm_content=Connectors%20&amp;%20Interconnects&amp;gclid=CjwKCAiA3uDwBRBFEiwA1VsajFpRq2OjG4RmtuGXWOX3NBMJTcv1glxE23z1SpbbgeTgjMK5AdF2YRoC3S4QAvD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 Q7 Q8 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1099,15 +1096,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="15.578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.83984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.89453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.3125" customWidth="1"/>
@@ -1132,13 +1130,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1158,13 +1156,13 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1184,13 +1182,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1207,16 +1205,16 @@
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1236,13 +1234,13 @@
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1262,13 +1260,13 @@
         <v>23</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1288,13 +1286,13 @@
         <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1317,10 +1315,10 @@
         <v>32</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1340,13 +1338,13 @@
         <v>36</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1366,233 +1364,164 @@
         <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>5</v>
       </c>
       <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
+      <c r="D14" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H15" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>560</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D17" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>560</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
+      <c r="E17" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://www.digikey.com/product-detail/en/sparkfun-electronics/BOB-13263/1568-1720-ND/7675364?utm_adgroup=DEV+Boards&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Development%20Boards%2C%20Kits%2C%20Programmers&amp;utm_term=&amp;utm_content=DEV+Boards&amp;gclid=CjwKCAiA3uDwBRBFEiwA1VsajG8ZEU__rDO9vt75xZ_ZmVJpdzuR2nNYhmOuDHuQax7VeKlEBKAZyxoCcLwQAvD_BwE"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="G5" r:id="rId6"/>
-    <hyperlink ref="G4" r:id="rId7"/>
-    <hyperlink ref="E6" r:id="rId8"/>
-    <hyperlink ref="F6" r:id="rId9"/>
-    <hyperlink ref="G6" r:id="rId10"/>
-    <hyperlink ref="E7" r:id="rId11"/>
-    <hyperlink ref="F7" r:id="rId12"/>
-    <hyperlink ref="G7" r:id="rId13"/>
-    <hyperlink ref="E8" r:id="rId14"/>
-    <hyperlink ref="F8" r:id="rId15"/>
-    <hyperlink ref="E9" r:id="rId16"/>
-    <hyperlink ref="F9" r:id="rId17"/>
-    <hyperlink ref="G9" r:id="rId18"/>
-    <hyperlink ref="E10" r:id="rId19"/>
-    <hyperlink ref="F10" r:id="rId20"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://www.digikey.com/product-detail/en/sparkfun-electronics/BOB-13263/1568-1720-ND/7675364?utm_adgroup=DEV+Boards&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Development%20Boards%2C%20Kits%2C%20Programmers&amp;utm_term=&amp;utm_content=DEV+Boards&amp;gclid=CjwKCAiA3uDwBRBFEiwA1VsajG8ZEU__rDO9vt75xZ_ZmVJpdzuR2nNYhmOuDHuQax7VeKlEBKAZyxoCcLwQAvD_BwE" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G7" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F8" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F9" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G9" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E10" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F10" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId21"/>

</xml_diff>